<commit_message>
Menage d'une fonction inutilisée
Former-commit-id: 50d48ebbd6eb9ba1e84b9171847e64b512235770
</commit_message>
<xml_diff>
--- a/documentation/3 - Réalisation/Client's request map.xlsx
+++ b/documentation/3 - Réalisation/Client's request map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="212">
   <si>
     <t>File path</t>
   </si>
@@ -736,19 +736,10 @@
     <t>Ext.Panel.getLoader().load()</t>
   </si>
   <si>
-    <t>ajaxgetchildren</t>
-  </si>
-  <si>
     <t>get-map-parameters</t>
   </si>
   <si>
     <t>show-add-data</t>
-  </si>
-  <si>
-    <t>proxy</t>
-  </si>
-  <si>
-    <t>getfeatureinfo</t>
   </si>
   <si>
     <t>"js": [
@@ -792,6 +783,9 @@
   </si>
   <si>
     <t>Gets the map parameters</t>
+  </si>
+  <si>
+    <t>a compléter (l'url est renvoyée depuis le serveur)</t>
   </si>
 </sst>
 </file>
@@ -833,7 +827,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -852,6 +846,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -866,7 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -877,6 +877,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1181,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D41" sqref="C41:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2112,10 +2116,10 @@
         <v>126</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E23" t="s">
         <v>111</v>
@@ -2153,10 +2157,10 @@
         <v>127</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E24" t="s">
         <v>111</v>
@@ -2194,10 +2198,10 @@
         <v>128</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E25" t="s">
         <v>111</v>
@@ -2229,19 +2233,19 @@
     </row>
     <row r="26" spans="1:13" ht="390" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B26" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C26" t="s">
         <v>151</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
@@ -2265,7 +2269,7 @@
         <v>13</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="285" x14ac:dyDescent="0.25">
@@ -2688,7 +2692,7 @@
       <c r="C37" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="8" t="s">
         <v>168</v>
       </c>
       <c r="E37" t="s">
@@ -2717,6 +2721,23 @@
       </c>
       <c r="M37" s="3" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" t="s">
+        <v>200</v>
+      </c>
+      <c r="C38" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2726,34 +2747,19 @@
       <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>203</v>
-      </c>
+      <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="C42" t="s">
-        <v>161</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>205</v>
-      </c>
+      <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
-      <c r="C43" t="s">
-        <v>206</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>207</v>
-      </c>
+      <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D44" s="6"/>

</xml_diff>

<commit_message>
Ajout de la nouvelle requête au fichier "Client's request map"
Former-commit-id: 362e0dcccc2e119eb9efa52e312255d12c3c2242
</commit_message>
<xml_diff>
--- a/documentation/3 - Réalisation/Client's request map.xlsx
+++ b/documentation/3 - Réalisation/Client's request map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="218">
   <si>
     <t>File path</t>
   </si>
@@ -786,6 +786,29 @@
   </si>
   <si>
     <t>a compléter (l'url est renvoyée depuis le serveur)</t>
+  </si>
+  <si>
+    <t>website\htdocs\client\ogamDesktop\app\ux\request\AdvancedRequestFieldSet.js</t>
+  </si>
+  <si>
+    <t>ajaxgetqueryformfields</t>
+  </si>
+  <si>
+    <t>Gets the dataset's query forms criteria / columns</t>
+  </si>
+  <si>
+    <t>OgamDesktop.model.request.fieldset.Criterion
+OgamDesktop.model.request.fieldset.Columns</t>
+  </si>
+  <si>
+    <t>query:plot
+page:1
+start:0
+limit:3
+filter:[{"property":"processId","value":"SPECIES"},{"property":"form","value":"PLOT_FORM"},{"property":"fieldsType","value":"criteria"}]</t>
+  </si>
+  <si>
+    <t>{"total":2, "root":[{"inputType":"TEXT","isCriteria":"1","isResult":"1","isDefaultCriteria":"0","isDefaultResult":"1","defaultValue":null,"decimals":null,"mask":null,"editable":null,"insertable":null,"isPK":null,"required":null,"position":2,"data":"PLOT_CODE","format":"PLOT_FORM","label":"Plot code","unit":"PLOT_CODE","type":"STRING","subtype":null,"definition":"The identifier of the plot for the country","value":null,"valueLabel":null},{"inputType":"CHECKBOX","isCriteria":"1","isResult":"1","isDefaultCriteria":"1","isDefaultResult":"1","defaultValue":"1","decimals":null,"mask":null,"editable":null,"insertable":null,"isPK":null,"required":null,"position":5,"data":"IS_FOREST_PLOT","format":"PLOT_FORM","label":"Is a forest plot","unit":"IS_FOREST_PLOT","type":"STRING","subtype":null,"definition":"True if the plot is a forest plot","value":null,"valueLabel":null}]}</t>
   </si>
 </sst>
 </file>
@@ -1183,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D41" sqref="C41:D41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,10 +1222,10 @@
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="37.7109375" customWidth="1"/>
-    <col min="9" max="9" width="44" customWidth="1"/>
+    <col min="9" max="9" width="46.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="42.85546875" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="76.28515625" customWidth="1"/>
     <col min="13" max="13" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1575,18 +1598,18 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>132</v>
+    <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>212</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>214</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>63</v>
+        <v>213</v>
       </c>
       <c r="E10" t="s">
         <v>51</v>
@@ -1600,34 +1623,34 @@
       <c r="H10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I10" t="s">
-        <v>66</v>
+      <c r="I10" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="J10" t="s">
         <v>25</v>
       </c>
       <c r="K10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10" t="s">
-        <v>70</v>
+        <v>25</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="M10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
         <v>51</v>
@@ -1642,33 +1665,33 @@
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J11" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="K11" t="s">
         <v>45</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>49</v>
+      <c r="L11" t="s">
+        <v>70</v>
       </c>
       <c r="M11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>73</v>
+      <c r="A12" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
         <v>51</v>
@@ -1677,39 +1700,39 @@
         <v>27</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="J12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K12" t="s">
         <v>45</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="M12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
         <v>51</v>
@@ -1718,25 +1741,25 @@
         <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="K13" t="s">
         <v>45</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="M13" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1750,7 +1773,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
         <v>51</v>
@@ -1774,24 +1797,24 @@
         <v>45</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
         <v>51</v>
@@ -1815,24 +1838,24 @@
         <v>45</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="M15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>134</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
         <v>51</v>
@@ -1841,39 +1864,39 @@
         <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I16" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="J16" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="K16" t="s">
         <v>45</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="M16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>79</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
         <v>51</v>
@@ -1882,39 +1905,39 @@
         <v>27</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I17" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="J17" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="K17" t="s">
         <v>45</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="M17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
         <v>51</v>
@@ -1938,109 +1961,109 @@
         <v>45</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="D19" t="s">
-        <v>104</v>
+      <c r="D19" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G19" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>136</v>
+        <v>26</v>
       </c>
       <c r="I19" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="J19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K19" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="M19" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>107</v>
+      <c r="D20" t="s">
+        <v>104</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="F20" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G20" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>26</v>
+        <v>136</v>
       </c>
       <c r="I20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s">
-        <v>110</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
         <v>27</v>
@@ -2058,39 +2081,39 @@
         <v>25</v>
       </c>
       <c r="K21" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="M21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>110</v>
       </c>
       <c r="F22" t="s">
         <v>27</v>
       </c>
       <c r="G22" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="I22" t="s">
         <v>25</v>
@@ -2102,27 +2125,27 @@
         <v>23</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="M22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>209</v>
+        <v>118</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
         <v>27</v>
@@ -2131,7 +2154,7 @@
         <v>16</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I23" t="s">
         <v>25</v>
@@ -2140,21 +2163,21 @@
         <v>25</v>
       </c>
       <c r="K23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
+      </c>
+      <c r="M23" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>208</v>
@@ -2184,18 +2207,18 @@
         <v>25</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>208</v>
@@ -2225,106 +2248,106 @@
         <v>25</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="390" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>206</v>
+        <v>114</v>
       </c>
       <c r="B26" t="s">
-        <v>210</v>
-      </c>
-      <c r="C26" t="s">
-        <v>151</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>205</v>
+        <v>128</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E26" t="s">
+        <v>111</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G26" t="s">
         <v>16</v>
       </c>
-      <c r="H26" t="s">
-        <v>14</v>
+      <c r="H26" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="I26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K26" t="s">
-        <v>24</v>
-      </c>
-      <c r="L26" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="285" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>170</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="390" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>206</v>
       </c>
       <c r="B27" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="C27" t="s">
         <v>151</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E27" t="s">
-        <v>51</v>
+      <c r="D27" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="F27" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>172</v>
+        <v>16</v>
+      </c>
+      <c r="H27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" t="s">
+        <v>24</v>
       </c>
       <c r="K27" t="s">
-        <v>45</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>49</v>
+        <v>24</v>
+      </c>
+      <c r="L27" t="s">
+        <v>13</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>152</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="285" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="B28" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C28" t="s">
         <v>151</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E28" t="s">
         <v>51</v>
@@ -2338,11 +2361,11 @@
       <c r="H28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I28" t="s">
-        <v>173</v>
-      </c>
-      <c r="J28" t="s">
-        <v>174</v>
+      <c r="I28" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="K28" t="s">
         <v>45</v>
@@ -2350,22 +2373,22 @@
       <c r="L28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M28" t="s">
-        <v>175</v>
+      <c r="M28" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C29" t="s">
         <v>151</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E29" t="s">
         <v>51</v>
@@ -2380,10 +2403,10 @@
         <v>26</v>
       </c>
       <c r="I29" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J29" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K29" t="s">
         <v>45</v>
@@ -2392,115 +2415,115 @@
         <v>49</v>
       </c>
       <c r="M29" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C30" t="s">
         <v>151</v>
       </c>
-      <c r="D30" t="s">
-        <v>156</v>
+      <c r="D30" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="E30" t="s">
-        <v>182</v>
+        <v>51</v>
       </c>
       <c r="F30" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G30" t="s">
         <v>43</v>
       </c>
       <c r="H30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" t="s">
+        <v>177</v>
+      </c>
+      <c r="J30" t="s">
+        <v>178</v>
+      </c>
+      <c r="K30" t="s">
+        <v>45</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" t="s">
+        <v>182</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="I30" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30" t="s">
-        <v>24</v>
-      </c>
-      <c r="K30" t="s">
-        <v>24</v>
-      </c>
-      <c r="L30" s="3" t="s">
+      <c r="I31" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="M30" s="3" t="s">
+      <c r="M31" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>157</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>190</v>
-      </c>
-      <c r="C31" t="s">
-        <v>161</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="E31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" t="s">
-        <v>24</v>
-      </c>
-      <c r="J31" t="s">
-        <v>24</v>
-      </c>
-      <c r="K31" t="s">
-        <v>24</v>
-      </c>
-      <c r="L31" t="s">
-        <v>13</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>158</v>
-      </c>
-      <c r="B32" t="s">
-        <v>187</v>
       </c>
       <c r="C32" t="s">
         <v>161</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E32" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="F32" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="I32" t="s">
         <v>24</v>
@@ -2509,48 +2532,48 @@
         <v>24</v>
       </c>
       <c r="K32" t="s">
-        <v>25</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="L32" t="s">
+        <v>13</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>45</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C33" t="s">
         <v>161</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="F33" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G33" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="I33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K33" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>45</v>
@@ -2559,18 +2582,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>159</v>
       </c>
       <c r="B34" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C34" t="s">
         <v>161</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E34" t="s">
         <v>51</v>
@@ -2594,33 +2617,33 @@
         <v>45</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="M34" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C35" t="s">
         <v>161</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E35" t="s">
-        <v>182</v>
+        <v>51</v>
       </c>
       <c r="F35" t="s">
         <v>27</v>
       </c>
       <c r="G35" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>26</v>
@@ -2632,71 +2655,71 @@
         <v>25</v>
       </c>
       <c r="K35" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="M35" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="B36" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C36" t="s">
         <v>161</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E36" t="s">
-        <v>18</v>
+        <v>182</v>
       </c>
       <c r="F36" t="s">
         <v>27</v>
       </c>
       <c r="G36" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K36" t="s">
         <v>23</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B37" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C37" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>168</v>
+      <c r="D37" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="E37" t="s">
-        <v>202</v>
+        <v>18</v>
       </c>
       <c r="F37" t="s">
         <v>27</v>
@@ -2714,16 +2737,16 @@
         <v>24</v>
       </c>
       <c r="K37" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>197</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>160</v>
       </c>
@@ -2733,21 +2756,56 @@
       <c r="C38" t="s">
         <v>161</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" t="s">
+        <v>202</v>
+      </c>
+      <c r="F38" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I38" t="s">
+        <v>24</v>
+      </c>
+      <c r="J38" t="s">
+        <v>24</v>
+      </c>
+      <c r="K38" t="s">
+        <v>45</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" t="s">
+        <v>200</v>
+      </c>
+      <c r="C39" t="s">
+        <v>161</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E39" s="9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L40" s="4"/>
-    </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="6"/>
+      <c r="L41" s="4"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -2762,7 +2820,13 @@
       <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
       <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D45" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
OGAM-424 API JSON , docs
Former-commit-id: b9b249abce400152b7614e5429c44da07028cdd4
</commit_message>
<xml_diff>
--- a/documentation/3 - Réalisation/Client's request map.xlsx
+++ b/documentation/3 - Réalisation/Client's request map.xlsx
@@ -337,9 +337,6 @@
 node:*</t>
   </si>
   <si>
-    <t>[{"text":"Vivant","id":"349525","vernacularName":null,"isReference":"1"}]</t>
-  </si>
-  <si>
     <t>Gets the children nodes of a taxref node</t>
   </si>
   <si>
@@ -507,9 +504,6 @@
     <t>id:SCHEMA/RAW_DATA/FORMAT/PLOT_DATA/PROVIDER_ID/1/PLOT_CODE/01575-14060-4-0T/CYCLE/5</t>
   </si>
   <si>
-    <t>{"formats":[{"title":"Localisation","children_count":1,"id":"SCHEMA\/RAW_DATA\/FORMAT\/LOCATION_DATA\/PROVIDER_ID\/1\/PLOT_CODE\/01575-14060-4-0T","fields":[{"label":"Commune","value":["CORMORANCHE-SUR-SAONE (01123)","GARNERANS (01167)"],"inputType":"SELECT","type":"ARRAY"},{"label":"D\u00e9partement","value":"AIN","inputType":"SELECT","type":"CODE"}],"editURL":"SCHEMA\/RAW_DATA\/FORMAT\/LOCATION_DATA\/PROVIDER_ID\/1\/PLOT_CODE\/01575-14060-4-0T"},{"title":"Donn\u00e9es du point","children_count":0,"id":"SCHEMA\/RAW_DATA\/FORMAT\/PLOT_DATA\/PROVIDER_ID\/1\/PLOT_CODE\/01575-14060-4-0T\/CYCLE\/5","fields":[{"label":"Identifiant du fournisseur de donn\u00e9es","value":"France","inputType":"SELECT","type":"CODE"},{"label":"Code du point","value":"01575-14060-4-0T","inputType":"TEXT","type":"STRING"},{"label":"Cycle","value":"5","inputType":"TEXT","type":"STRING"},{"label":"Date d'inventaire","value":"2007\/11\/27","inputType":"DATE","type":"DATE"},{"label":"Est un point for\u00eat","value":"1","inputType":"CHECKBOX","type":"STRING"},{"label":"Corine biotope","value":["Habitats littoraux et halophiles"],"inputType":"TREE","type":"ARRAY"},{"label":"Commentaire","value":"test data plot","inputType":"TEXT","type":"STRING"}],"editURL":"SCHEMA\/RAW_DATA\/FORMAT\/PLOT_DATA\/PROVIDER_ID\/1\/PLOT_CODE\/01575-14060-4-0T\/CYCLE\/5"}],"title":"Donn\u00e9es du point (1_01575-14060-4-0T_5)","maps1":{"title":"image","urls":[{"url":"http:\/\/wxs-i.ign.fr\/7gr31kqe5xttprd2g7zbkqgo\/geoportail\/r\/wms?LAYERS=ORTHOIMAGERY.ORTHOPHOTOS&amp;TRANSPARENT=true&amp;FORMAT=image%2Fpng&amp;SERVICE=WMS&amp;VERSION=1.3.0&amp;REQUEST=GetMap&amp;STYLES=&amp;BBOX=531065.24180649,5812149.7543612,541065.24180649,5822149.7543612&amp;WIDTH=300&amp;HEIGHT=300&amp;map.scalebar=STATUS+embed&amp;SESSION_ID=mlk6a2jgaij2vmqtv0n4njcruvaoj7qj&amp;PROVIDER_ID=1&amp;PLOT_CODE=01575-14060-4-0T&amp;CRS=EPSG%3A3857"},{"url":"http:\/\/localhost\/mapserv-ogam?LAYERS=result_location&amp;TRANSPARENT=true&amp;FORMAT=image%2Fpng&amp;SERVICE=WMS&amp;VERSION=1.1.1&amp;REQUEST=GetMap&amp;STYLES=&amp;BBOX=531065.24180649,5812149.7543612,541065.24180649,5822149.7543612&amp;WIDTH=300&amp;HEIGHT=300&amp;map.scalebar=STATUS+embed&amp;SESSION_ID=mlk6a2jgaij2vmqtv0n4njcruvaoj7qj&amp;PROVIDER_ID=1&amp;PLOT_CODE=01575-14060-4-0T&amp;SRS=EPSG%3A3857"}]},"maps2":{"title":"overview","urls":[{"url":"http:\/\/wxs-i.ign.fr\/7gr31kqe5xttprd2g7zbkqgo\/geoportail\/r\/wms?LAYERS=ORTHOIMAGERY.ORTHOPHOTOS&amp;TRANSPARENT=true&amp;FORMAT=image%2Fpng&amp;SERVICE=WMS&amp;VERSION=1.3.0&amp;REQUEST=GetMap&amp;STYLES=&amp;BBOX=436065.24180649,5717149.7543612,636065.24180649,5917149.7543612&amp;WIDTH=300&amp;HEIGHT=300&amp;map.scalebar=STATUS+embed&amp;SESSION_ID=mlk6a2jgaij2vmqtv0n4njcruvaoj7qj&amp;PROVIDER_ID=1&amp;PLOT_CODE=01575-14060-4-0T&amp;CRS=EPSG%3A3857"},{"url":"http:\/\/www.ogam.fr\/mapProxy.php?LAYERS=nuts_0&amp;TRANSPARENT=true&amp;FORMAT=image%2Fpng&amp;SERVICE=WMS&amp;VERSION=1.1.1&amp;REQUEST=GetMap&amp;STYLES=&amp;BBOX=436065.24180649,5717149.7543612,636065.24180649,5917149.7543612&amp;WIDTH=300&amp;HEIGHT=300&amp;map.scalebar=STATUS+embed&amp;SESSION_ID=mlk6a2jgaij2vmqtv0n4njcruvaoj7qj&amp;PROVIDER_ID=1&amp;PLOT_CODE=01575-14060-4-0T&amp;SRS=EPSG%3A3857"},{"url":"http:\/\/localhost\/mapserv-ogam?LAYERS=plot_location_detail&amp;TRANSPARENT=true&amp;FORMAT=image%2Fpng&amp;SERVICE=WMS&amp;VERSION=1.1.1&amp;REQUEST=GetMap&amp;STYLES=&amp;BBOX=436065.24180649,5717149.7543612,636065.24180649,5917149.7543612&amp;WIDTH=300&amp;HEIGHT=300&amp;map.scalebar=STATUS+embed&amp;SESSION_ID=mlk6a2jgaij2vmqtv0n4njcruvaoj7qj&amp;PROVIDER_ID=1&amp;PLOT_CODE=01575-14060-4-0T&amp;SRS=EPSG%3A3857"}]}}</t>
-  </si>
-  <si>
     <t>Gets a pdf export of the detail panel</t>
   </si>
   <si>
@@ -549,12 +543,6 @@
     <t>DOC (PDF)</t>
   </si>
   <si>
-    <t>[{"text":"Habitats littoraux et halophiles","id":"1"},{"text":"Milieux aquatiques non marins","id":"2"},{"text":"Landes, frutic\u00e9es, pelouses et prairies","id":"3"},{"text":"For\u00eats","id":"4"},{"text":"Tourbi\u00e8res et marais","id":"5"},{"text":"Rochers continentaux, \u00e9boulis et sables","id":"6"},{"text":"Terres agricoles et paysages artificiels","id":"8"}]</t>
-  </si>
-  <si>
-    <t>[ {"id":"SPECIES","label":"Informations sur les esp\u00e8ces","definition":"Informations sur les donn\u00e9es des esp\u00e8ces","is_default":"1"},{"id":"TREES","label":"D\u00e9tails sur les arbres","definition":"D\u00e9tails sur les donn\u00e9es de chaque arbre","is_default":"0"}]</t>
-  </si>
-  <si>
     <t>ajaxgetlayers</t>
   </si>
   <si>
@@ -610,9 +598,6 @@
   </si>
   <si>
     <t>show-edit-data</t>
-  </si>
-  <si>
-    <t>{"services":[{"name":"geoportal_wmts", "config":{"urls": ["http://wxs-i.ign.fr/7gr31kqe5xttprd2g7zbkqgo/geoportail/wmts?"],"params":{"SERVICE":"WMTS","VERSION":"1.0.0","REQUEST":"getTile","style":"normal","matrixSet":"PM","requestEncoding":"KVP","maxExtent":[-20037508, -20037508, 20037508, 20037508],"serverResolutions":[156543.033928,78271.516964,39135.758482,19567.879241,9783.939621,4891.969810,2445.984905,1222.992453,611.496226,305.748113,152.874057,76.437028,38.218514,19.109257,9.554629,4.777302,2.388657,1.194329,0.597164,0.298582,0.149291,0.074646],"tileOrigin":[-20037508,20037508]}}},{"name":"mapProxy_wfs", "config":{"urls":["http://www.ogam.fr/mapProxy.php?"],"params":{"SERVICE":"WFS","VERSION":"1.1.0","REQUEST":"GetFeature"}}},{"name":"geoportal_wms", "config":{"urls":["http://wxs-i.ign.fr/7gr31kqe5xttprd2g7zbkqgo/geoportail/r/wms?"],"params":{"SERVICE":"WMS","VERSION":"1.3.0","REQUEST":"GetMap"}}},{"name":"legend_mapProxy", "config":{"urls":["http://www.ogam.fr/mapProxy.php?"],"params":{"SERVICE":"WMS","VERSION":"1.1.1","REQUEST":"GetLegendGraphic"}}},{"name":"proxy_wfs", "config":{"urls":["http://www.ogam.fr/proxy/getwfs?"],"params":{"SERVICE":"WFS","VERSION":"1.0.0","REQUEST":"GetFeature"}}},{"name":"local_mapserver", "config":{"urls":["http://localhost/mapserv-ogam?"],"params":{"SERVICE":"WMS","VERSION":"1.1.1","REQUEST":"GetMap"}}},{"name":"mapProxy", "config":{"urls":["http://www.ogam.fr/mapProxy.php?"],"params":{"SERVICE":"WMS","VERSION":"1.1.1","REQUEST":"GetMap"}}}],"layers":[{"singleTile":false, "name":"nuts_0", "viewServiceName":"mapProxy", "featureServiceName":"mapProxy_wfs", "legendServiceName":"legend_mapProxy", "params":{"layers" : ["nuts_0"], "transparent": true, "format": "image/PNG", "isHidden": false, "isDisabled": false, "isChecked": true, "activateType": "NONE", "hasSLD": false, "session_id": "mlk6a2jgaij2vmqtv0n4njcruvaoj7qj", "provider_id": "1"}, "options":{"buffer": 0, "nodeGroup": "6", "transitionEffect": "resize", "visibility": true, "isBaseLayer": false, "opacity": 1,"label":"Frontières", "resolutions": [8819.439681947, 3527.7758727788, 1763.8879363894, 881.9439681947, 352.77758727788, 176.38879363894]}},{"singleTile":false, "name":"plot_location_detail", "viewServiceName":"mapProxy", "featureServiceName":"", "legendServiceName":"", "params":{"layers" : ["plot_location_detail"], "transparent": true, "format": "image/PNG", "isHidden": true, "isDisabled": false, "isChecked": false, "activateType": "NONE", "hasSLD": false, "session_id": "mlk6a2jgaij2vmqtv0n4njcruvaoj7qj", "provider_id": "1"}, "options":{"buffer": 0, "nodeGroup": "-1", "visibility": false, "isBaseLayer": false, "opacity": 1,"label":"Détails sur les localisations"}},{"singleTile":true, "name":"all_locations", "viewServiceName":"mapProxy", "featureServiceName":"mapProxy_wfs", "legendServiceName":"legend_mapProxy", "params":{"layers" : ["all_locations"], "transparent": true, "format": "image/PNG", "isHidden": false, "isDisabled": false, "isChecked": true, "activateType": "NONE", "hasSLD": false, "session_id": "mlk6a2jgaij2vmqtv0n4njcruvaoj7qj", "provider_id": "1"}, "options":{"buffer": 0, "nodeGroup": "-1", "visibility": true, "isBaseLayer": false, "opacity": 1,"label":"Localisations"}},{"singleTile":false, "name":"ORTHOIMAGERY.ORTHOPHOTOS", "viewServiceName":"geoportal_wmts", "featureServiceName":"", "legendServiceName":"", "params":{"layers" : ["ORTHOIMAGERY.ORTHOPHOTOS"], "transparent": true, "format": "image/jpeg", "isHidden": false, "isDisabled": false, "isChecked": false, "activateType": "NONE", "hasSLD": false, "session_id": "mlk6a2jgaij2vmqtv0n4njcruvaoj7qj", "provider_id": "1"}, "options":{"buffer": 0, "nodeGroup": "-1", "transitionEffect": "resize", "visibility": false, "isBaseLayer": false, "opacity": "0.5","label":"BD Ortho"}},{"singleTile":true, "name":"result_location", "viewServiceName":"mapProxy", "featureServiceName":"", "legendServiceName":"legend_mapProxy", "params":{"layers" : ["result_location"], "transparent": true, "format": "image/PNG", "isHidden": false, "isDisabled": true, "isChecked": false, "activateType": "REQUEST", "hasSLD": false, "session_id": "mlk6a2jgaij2vmqtv0n4njcruvaoj7qj", "provider_id": "1"}, "options":{"buffer": 0, "nodeGroup": "-1", "visibility": false, "isBaseLayer": false, "opacity": 1,"label":"Results"}}]}</t>
   </si>
   <si>
     <t>website\htdocs\client\ogamDesktop\app\store\map\Layer.js
@@ -631,9 +616,6 @@
   </si>
   <si>
     <t>OgamDesktop.store.map.LayerNode</t>
-  </si>
-  <si>
-    <t>[{"text": "Fonds", "expanded": true, "checked": false, "hidden": false, "disabled": false, "leaf": false, "nodeType" : "gx_layercontainer", "nodeGroup": "6" }, {"text": "BD Ortho", "expanded": false, "checked": false, "hidden": false, "disabled": false, "leaf": true, "nodeType" : "gx_layer", "layer": "ORTHOIMAGERY.ORTHOPHOTOS" }, {"text": "Results", "expanded": false, "checked": false, "hidden": false, "disabled": true, "leaf": true, "nodeType" : "gx_layer", "layer": "result_location" }, {"text": "Localisations", "expanded": false, "checked": true, "hidden": false, "disabled": false, "leaf": true, "nodeType" : "gx_layer", "layer": "all_locations" }, {"text": "Détails sur les localisations", "expanded": false, "checked": false, "hidden": true, "disabled": false, "leaf": true, "nodeType" : "gx_layer", "layer": "plot_location_detail" }]</t>
   </si>
   <si>
     <t>Gets the layers tree nodes</t>
@@ -808,7 +790,25 @@
 filter:[{"property":"processId","value":"SPECIES"},{"property":"form","value":"PLOT_FORM"},{"property":"fieldsType","value":"criteria"}]</t>
   </si>
   <si>
-    <t>{"total":2, "root":[{"inputType":"TEXT","isCriteria":"1","isResult":"1","isDefaultCriteria":"0","isDefaultResult":"1","defaultValue":null,"decimals":null,"mask":null,"editable":null,"insertable":null,"isPK":null,"required":null,"position":2,"data":"PLOT_CODE","format":"PLOT_FORM","label":"Plot code","unit":"PLOT_CODE","type":"STRING","subtype":null,"definition":"The identifier of the plot for the country","value":null,"valueLabel":null},{"inputType":"CHECKBOX","isCriteria":"1","isResult":"1","isDefaultCriteria":"1","isDefaultResult":"1","defaultValue":"1","decimals":null,"mask":null,"editable":null,"insertable":null,"isPK":null,"required":null,"position":5,"data":"IS_FOREST_PLOT","format":"PLOT_FORM","label":"Is a forest plot","unit":"IS_FOREST_PLOT","type":"STRING","subtype":null,"definition":"True if the plot is a forest plot","value":null,"valueLabel":null}]}</t>
+    <t>{"success":true,"services":[{"name":"geoportal_wmts", "config":{"urls": ["http://wxs-i.ign.fr/7gr31kqe5xttprd2g7zbkqgo/geoportail/wmts?"],"params":{"SERVICE":"WMTS","VERSION":"1.0.0","REQUEST":"getTile","style":"normal","matrixSet":"PM","requestEncoding":"KVP","maxExtent":[-20037508, -20037508, 20037508, 20037508],"serverResolutions":[156543.033928,78271.516964,39135.758482,19567.879241,9783.939621,4891.969810,2445.984905,1222.992453,611.496226,305.748113,152.874057,76.437028,38.218514,19.109257,9.554629,4.777302,2.388657,1.194329,0.597164,0.298582,0.149291,0.074646],"tileOrigin":[-20037508,20037508]}}},{"name":"mapProxy_wfs", "config":{"urls":["http://www.ogam.fr/mapProxy.php?"],"params":{"SERVICE":"WFS","VERSION":"1.1.0","REQUEST":"GetFeature"}}},{"name":"geoportal_wms", "config":{"urls":["http://wxs-i.ign.fr/7gr31kqe5xttprd2g7zbkqgo/geoportail/r/wms?"],"params":{"SERVICE":"WMS","VERSION":"1.3.0","REQUEST":"GetMap"}}},{"name":"legend_mapProxy", "config":{"urls":["http://www.ogam.fr/mapProxy.php?"],"params":{"SERVICE":"WMS","VERSION":"1.1.1","REQUEST":"GetLegendGraphic"}}},{"name":"proxy_wfs", "config":{"urls":["http://www.ogam.fr/proxy/getwfs?"],"params":{"SERVICE":"WFS","VERSION":"1.0.0","REQUEST":"GetFeature"}}},{"name":"local_mapserver", "config":{"urls":["http://localhost/mapserv-ogam?"],"params":{"SERVICE":"WMS","VERSION":"1.1.1","REQUEST":"GetMap"}}},{"name":"mapProxy", "config":{"urls":["http://www.ogam.fr/mapProxy.php?"],"params":{"SERVICE":"WMS","VERSION":"1.1.1","REQUEST":"GetMap"}}}],"layers":[{"singleTile":false, "name":"nuts_0", "viewServiceName":"mapProxy", "featureServiceName":"mapProxy_wfs", "legendServiceName":"legend_mapProxy", "params":{"layers" : ["nuts_0"], "transparent": true, "format": "image/PNG", "isHidden": false, "isDisabled": false, "isChecked": true, "activateType": "NONE", "hasSLD": false, "session_id": "mlk6a2jgaij2vmqtv0n4njcruvaoj7qj", "provider_id": "1"}, "options":{"buffer": 0, "nodeGroup": "6", "transitionEffect": "resize", "visibility": true, "isBaseLayer": false, "opacity": 1,"label":"Frontières", "resolutions": [8819.439681947, 3527.7758727788, 1763.8879363894, 881.9439681947, 352.77758727788, 176.38879363894]}},{"singleTile":false, "name":"plot_location_detail", "viewServiceName":"mapProxy", "featureServiceName":"", "legendServiceName":"", "params":{"layers" : ["plot_location_detail"], "transparent": true, "format": "image/PNG", "isHidden": true, "isDisabled": false, "isChecked": false, "activateType": "NONE", "hasSLD": false, "session_id": "mlk6a2jgaij2vmqtv0n4njcruvaoj7qj", "provider_id": "1"}, "options":{"buffer": 0, "nodeGroup": "-1", "visibility": false, "isBaseLayer": false, "opacity": 1,"label":"Détails sur les localisations"}},{"singleTile":true, "name":"all_locations", "viewServiceName":"mapProxy", "featureServiceName":"mapProxy_wfs", "legendServiceName":"legend_mapProxy", "params":{"layers" : ["all_locations"], "transparent": true, "format": "image/PNG", "isHidden": false, "isDisabled": false, "isChecked": true, "activateType": "NONE", "hasSLD": false, "session_id": "mlk6a2jgaij2vmqtv0n4njcruvaoj7qj", "provider_id": "1"}, "options":{"buffer": 0, "nodeGroup": "-1", "visibility": true, "isBaseLayer": false, "opacity": 1,"label":"Localisations"}},{"singleTile":false, "name":"ORTHOIMAGERY.ORTHOPHOTOS", "viewServiceName":"geoportal_wmts", "featureServiceName":"", "legendServiceName":"", "params":{"layers" : ["ORTHOIMAGERY.ORTHOPHOTOS"], "transparent": true, "format": "image/jpeg", "isHidden": false, "isDisabled": false, "isChecked": false, "activateType": "NONE", "hasSLD": false, "session_id": "mlk6a2jgaij2vmqtv0n4njcruvaoj7qj", "provider_id": "1"}, "options":{"buffer": 0, "nodeGroup": "-1", "transitionEffect": "resize", "visibility": false, "isBaseLayer": false, "opacity": "0.5","label":"BD Ortho"}},{"singleTile":true, "name":"result_location", "viewServiceName":"mapProxy", "featureServiceName":"", "legendServiceName":"legend_mapProxy", "params":{"layers" : ["result_location"], "transparent": true, "format": "image/PNG", "isHidden": false, "isDisabled": true, "isChecked": false, "activateType": "REQUEST", "hasSLD": false, "session_id": "mlk6a2jgaij2vmqtv0n4njcruvaoj7qj", "provider_id": "1"}, "options":{"buffer": 0, "nodeGroup": "-1", "visibility": false, "isBaseLayer": false, "opacity": 1,"label":"Results"}}]}</t>
+  </si>
+  <si>
+    <t>{"success":true, "data":[ {"id":"SPECIES","label":"Informations sur les esp\u00e8ces","definition":"Informations sur les donn\u00e9es des esp\u00e8ces","is_default":"1"},{"id":"TREES","label":"D\u00e9tails sur les arbres","definition":"D\u00e9tails sur les donn\u00e9es de chaque arbre","is_default":"0"}]}</t>
+  </si>
+  <si>
+    <t>{"success":true,"total":2, "root":[{"inputType":"TEXT","isCriteria":"1","isResult":"1","isDefaultCriteria":"0","isDefaultResult":"1","defaultValue":null,"decimals":null,"mask":null,"editable":null,"insertable":null,"isPK":null,"required":null,"position":2,"data":"PLOT_CODE","format":"PLOT_FORM","label":"Plot code","unit":"PLOT_CODE","type":"STRING","subtype":null,"definition":"The identifier of the plot for the country","value":null,"valueLabel":null},{"inputType":"CHECKBOX","isCriteria":"1","isResult":"1","isDefaultCriteria":"1","isDefaultResult":"1","defaultValue":"1","decimals":null,"mask":null,"editable":null,"insertable":null,"isPK":null,"required":null,"position":5,"data":"IS_FOREST_PLOT","format":"PLOT_FORM","label":"Is a forest plot","unit":"IS_FOREST_PLOT","type":"STRING","subtype":null,"definition":"True if the plot is a forest plot","value":null,"valueLabel":null}]}</t>
+  </si>
+  <si>
+    <t>{"success":true, "data":[{"text":"Habitats littoraux et halophiles","id":"1"},{"text":"Milieux aquatiques non marins","id":"2"},{"text":"Landes, frutic\u00e9es, pelouses et prairies","id":"3"},{"text":"For\u00eats","id":"4"},{"text":"Tourbi\u00e8res et marais","id":"5"},{"text":"Rochers continentaux, \u00e9boulis et sables","id":"6"},{"text":"Terres agricoles et paysages artificiels","id":"8"}]}</t>
+  </si>
+  <si>
+    <t>{"success":true, "data":[{"text":"Vivant","id":"349525","vernacularName":null,"isReference":"1"}]}</t>
+  </si>
+  <si>
+    <t>{"success":true,"formats":[{"title":"Localisation","children_count":1,"id":"SCHEMA\/RAW_DATA\/FORMAT\/LOCATION_DATA\/PROVIDER_ID\/1\/PLOT_CODE\/01575-14060-4-0T","fields":[{"label":"Commune","value":["CORMORANCHE-SUR-SAONE (01123)","GARNERANS (01167)"],"inputType":"SELECT","type":"ARRAY"},{"label":"D\u00e9partement","value":"AIN","inputType":"SELECT","type":"CODE"}],"editURL":"SCHEMA\/RAW_DATA\/FORMAT\/LOCATION_DATA\/PROVIDER_ID\/1\/PLOT_CODE\/01575-14060-4-0T"},{"title":"Donn\u00e9es du point","children_count":0,"id":"SCHEMA\/RAW_DATA\/FORMAT\/PLOT_DATA\/PROVIDER_ID\/1\/PLOT_CODE\/01575-14060-4-0T\/CYCLE\/5","fields":[{"label":"Identifiant du fournisseur de donn\u00e9es","value":"France","inputType":"SELECT","type":"CODE"},{"label":"Code du point","value":"01575-14060-4-0T","inputType":"TEXT","type":"STRING"},{"label":"Cycle","value":"5","inputType":"TEXT","type":"STRING"},{"label":"Date d'inventaire","value":"2007\/11\/27","inputType":"DATE","type":"DATE"},{"label":"Est un point for\u00eat","value":"1","inputType":"CHECKBOX","type":"STRING"},{"label":"Corine biotope","value":["Habitats littoraux et halophiles"],"inputType":"TREE","type":"ARRAY"},{"label":"Commentaire","value":"test data plot","inputType":"TEXT","type":"STRING"}],"editURL":"SCHEMA\/RAW_DATA\/FORMAT\/PLOT_DATA\/PROVIDER_ID\/1\/PLOT_CODE\/01575-14060-4-0T\/CYCLE\/5"}],"title":"Donn\u00e9es du point (1_01575-14060-4-0T_5)","maps1":{"title":"image","urls":[{"url":"http:\/\/wxs-i.ign.fr\/7gr31kqe5xttprd2g7zbkqgo\/geoportail\/r\/wms?LAYERS=ORTHOIMAGERY.ORTHOPHOTOS&amp;TRANSPARENT=true&amp;FORMAT=image%2Fpng&amp;SERVICE=WMS&amp;VERSION=1.3.0&amp;REQUEST=GetMap&amp;STYLES=&amp;BBOX=531065.24180649,5812149.7543612,541065.24180649,5822149.7543612&amp;WIDTH=300&amp;HEIGHT=300&amp;map.scalebar=STATUS+embed&amp;SESSION_ID=mlk6a2jgaij2vmqtv0n4njcruvaoj7qj&amp;PROVIDER_ID=1&amp;PLOT_CODE=01575-14060-4-0T&amp;CRS=EPSG%3A3857"},{"url":"http:\/\/localhost\/mapserv-ogam?LAYERS=result_location&amp;TRANSPARENT=true&amp;FORMAT=image%2Fpng&amp;SERVICE=WMS&amp;VERSION=1.1.1&amp;REQUEST=GetMap&amp;STYLES=&amp;BBOX=531065.24180649,5812149.7543612,541065.24180649,5822149.7543612&amp;WIDTH=300&amp;HEIGHT=300&amp;map.scalebar=STATUS+embed&amp;SESSION_ID=mlk6a2jgaij2vmqtv0n4njcruvaoj7qj&amp;PROVIDER_ID=1&amp;PLOT_CODE=01575-14060-4-0T&amp;SRS=EPSG%3A3857"}]},"maps2":{"title":"overview","urls":[{"url":"http:\/\/wxs-i.ign.fr\/7gr31kqe5xttprd2g7zbkqgo\/geoportail\/r\/wms?LAYERS=ORTHOIMAGERY.ORTHOPHOTOS&amp;TRANSPARENT=true&amp;FORMAT=image%2Fpng&amp;SERVICE=WMS&amp;VERSION=1.3.0&amp;REQUEST=GetMap&amp;STYLES=&amp;BBOX=436065.24180649,5717149.7543612,636065.24180649,5917149.7543612&amp;WIDTH=300&amp;HEIGHT=300&amp;map.scalebar=STATUS+embed&amp;SESSION_ID=mlk6a2jgaij2vmqtv0n4njcruvaoj7qj&amp;PROVIDER_ID=1&amp;PLOT_CODE=01575-14060-4-0T&amp;CRS=EPSG%3A3857"},{"url":"http:\/\/www.ogam.fr\/mapProxy.php?LAYERS=nuts_0&amp;TRANSPARENT=true&amp;FORMAT=image%2Fpng&amp;SERVICE=WMS&amp;VERSION=1.1.1&amp;REQUEST=GetMap&amp;STYLES=&amp;BBOX=436065.24180649,5717149.7543612,636065.24180649,5917149.7543612&amp;WIDTH=300&amp;HEIGHT=300&amp;map.scalebar=STATUS+embed&amp;SESSION_ID=mlk6a2jgaij2vmqtv0n4njcruvaoj7qj&amp;PROVIDER_ID=1&amp;PLOT_CODE=01575-14060-4-0T&amp;SRS=EPSG%3A3857"},{"url":"http:\/\/localhost\/mapserv-ogam?LAYERS=plot_location_detail&amp;TRANSPARENT=true&amp;FORMAT=image%2Fpng&amp;SERVICE=WMS&amp;VERSION=1.1.1&amp;REQUEST=GetMap&amp;STYLES=&amp;BBOX=436065.24180649,5717149.7543612,636065.24180649,5917149.7543612&amp;WIDTH=300&amp;HEIGHT=300&amp;map.scalebar=STATUS+embed&amp;SESSION_ID=mlk6a2jgaij2vmqtv0n4njcruvaoj7qj&amp;PROVIDER_ID=1&amp;PLOT_CODE=01575-14060-4-0T&amp;SRS=EPSG%3A3857"}]}}</t>
+  </si>
+  <si>
+    <t>{"success":true,"layers":[{"text": "Fonds", "expanded": true, "checked": false, "hidden": false, "disabled": false, "leaf": false, "nodeType" : "gx_layercontainer", "nodeGroup": "6" }, {"text": "BD Ortho", "expanded": false, "checked": false, "hidden": false, "disabled": false, "leaf": true, "nodeType" : "gx_layer", "layer": "ORTHOIMAGERY.ORTHOPHOTOS" }, {"text": "Results", "expanded": false, "checked": false, "hidden": false, "disabled": true, "leaf": true, "nodeType" : "gx_layer", "layer": "result_location" }, {"text": "Localisations", "expanded": false, "checked": true, "hidden": false, "disabled": false, "leaf": true, "nodeType" : "gx_layer", "layer": "all_locations" }, {"text": "Détails sur les localisations", "expanded": false, "checked": false, "hidden": true, "disabled": false, "leaf": true, "nodeType" : "gx_layer", "layer": "plot_location_detail" }]}</t>
   </si>
 </sst>
 </file>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="F28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,7 +1308,7 @@
         <v>13</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
         <v>13</v>
       </c>
       <c r="M3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1390,7 +1390,7 @@
         <v>13</v>
       </c>
       <c r="M4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1431,7 +1431,7 @@
         <v>13</v>
       </c>
       <c r="M5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>13</v>
       </c>
       <c r="M6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1513,7 +1513,7 @@
         <v>13</v>
       </c>
       <c r="M7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1554,7 +1554,7 @@
         <v>49</v>
       </c>
       <c r="M8" t="s">
-        <v>149</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1600,16 +1600,16 @@
     </row>
     <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E10" t="s">
         <v>51</v>
@@ -1624,7 +1624,7 @@
         <v>26</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="J10" t="s">
         <v>25</v>
@@ -1633,15 +1633,15 @@
         <v>25</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="M10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
         <v>67</v>
@@ -1682,7 +1682,7 @@
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
         <v>68</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
         <v>55</v>
@@ -1923,7 +1923,7 @@
         <v>46</v>
       </c>
       <c r="M17" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -1972,7 +1972,7 @@
         <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -2005,24 +2005,24 @@
         <v>98</v>
       </c>
       <c r="M19" t="s">
-        <v>99</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" t="s">
         <v>104</v>
-      </c>
-      <c r="E20" t="s">
-        <v>105</v>
       </c>
       <c r="F20" t="s">
         <v>34</v>
@@ -2031,7 +2031,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I20" t="s">
         <v>24</v>
@@ -2043,24 +2043,24 @@
         <v>24</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
@@ -2084,27 +2084,27 @@
         <v>25</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M21" t="s">
-        <v>138</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" t="s">
         <v>109</v>
-      </c>
-      <c r="E22" t="s">
-        <v>110</v>
       </c>
       <c r="F22" t="s">
         <v>27</v>
@@ -2125,24 +2125,24 @@
         <v>23</v>
       </c>
       <c r="L22" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="M22" t="s">
         <v>129</v>
-      </c>
-      <c r="M22" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E23" t="s">
         <v>18</v>
@@ -2154,7 +2154,7 @@
         <v>16</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I23" t="s">
         <v>25</v>
@@ -2166,27 +2166,27 @@
         <v>23</v>
       </c>
       <c r="L23" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="M23" t="s">
         <v>115</v>
-      </c>
-      <c r="M23" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F24" t="s">
         <v>27</v>
@@ -2195,7 +2195,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I24" t="s">
         <v>25</v>
@@ -2207,27 +2207,27 @@
         <v>25</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F25" t="s">
         <v>27</v>
@@ -2236,7 +2236,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I25" t="s">
         <v>25</v>
@@ -2248,27 +2248,27 @@
         <v>25</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F26" t="s">
         <v>27</v>
@@ -2277,39 +2277,39 @@
         <v>16</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" t="s">
+        <v>25</v>
+      </c>
+      <c r="K26" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="I26" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" t="s">
-        <v>25</v>
-      </c>
-      <c r="K26" t="s">
-        <v>25</v>
-      </c>
-      <c r="L26" s="3" t="s">
+      <c r="M26" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="390" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B27" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
@@ -2333,21 +2333,21 @@
         <v>13</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="285" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E28" t="s">
         <v>51</v>
@@ -2362,10 +2362,10 @@
         <v>26</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K28" t="s">
         <v>45</v>
@@ -2374,21 +2374,21 @@
         <v>49</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B29" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E29" t="s">
         <v>51</v>
@@ -2403,10 +2403,10 @@
         <v>26</v>
       </c>
       <c r="I29" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="J29" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="K29" t="s">
         <v>45</v>
@@ -2415,21 +2415,21 @@
         <v>49</v>
       </c>
       <c r="M29" t="s">
-        <v>175</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B30" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>155</v>
       </c>
       <c r="E30" t="s">
         <v>51</v>
@@ -2444,10 +2444,10 @@
         <v>26</v>
       </c>
       <c r="I30" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="J30" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="K30" t="s">
         <v>45</v>
@@ -2456,24 +2456,24 @@
         <v>49</v>
       </c>
       <c r="M30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D31" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E31" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F31" t="s">
         <v>34</v>
@@ -2482,7 +2482,7 @@
         <v>43</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I31" t="s">
         <v>24</v>
@@ -2494,24 +2494,24 @@
         <v>24</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" t="s">
         <v>157</v>
       </c>
-      <c r="B32" t="s">
-        <v>190</v>
-      </c>
-      <c r="C32" t="s">
-        <v>161</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2538,24 +2538,24 @@
         <v>13</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E33" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F33" t="s">
         <v>34</v>
@@ -2584,16 +2584,16 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E34" t="s">
         <v>51</v>
@@ -2625,16 +2625,16 @@
     </row>
     <row r="35" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C35" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="E35" t="s">
         <v>51</v>
@@ -2658,27 +2658,27 @@
         <v>45</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="M35" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B36" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E36" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F36" t="s">
         <v>27</v>
@@ -2699,24 +2699,24 @@
         <v>23</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B37" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E37" t="s">
         <v>18</v>
@@ -2740,27 +2740,27 @@
         <v>23</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B38" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C38" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E38" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F38" t="s">
         <v>27</v>
@@ -2781,27 +2781,27 @@
         <v>45</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B39" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C39" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>